<commit_message>
Translation of p values
</commit_message>
<xml_diff>
--- a/p values.xlsx
+++ b/p values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\locl1\Documents\Laptop Drive\Toxicología Acuática\Tesis\Resultados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Código GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F4AE19-05F9-4016-8232-F8ECCC70AA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C1F084-CFF5-4A1B-BF17-CDAC278C696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{94F7DDCC-7829-401A-BE83-BFBA96EDE9FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{94F7DDCC-7829-401A-BE83-BFBA96EDE9FB}"/>
   </bookViews>
   <sheets>
     <sheet name="mortalidad_sedimento" sheetId="1" r:id="rId1"/>
@@ -201,19 +201,19 @@
     <t>S,C,1</t>
   </si>
   <si>
-    <t>A,1,2,3</t>
-  </si>
-  <si>
-    <t>A,✱</t>
-  </si>
-  <si>
-    <t>A,C,3,4</t>
-  </si>
-  <si>
-    <t>A,C,1,4</t>
-  </si>
-  <si>
-    <t>A,C,1</t>
+    <t>W,1,2,3</t>
+  </si>
+  <si>
+    <t>W,✱</t>
+  </si>
+  <si>
+    <t>W,C,3,4</t>
+  </si>
+  <si>
+    <t>W,C,1,4</t>
+  </si>
+  <si>
+    <t>W,C,1</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,8 +276,6 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,13 +619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35669C1-8FC8-4BE3-BDBF-A2B1FA1009E0}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C38" sqref="C38:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -649,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -657,7 +655,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -665,7 +663,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -673,7 +671,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -684,7 +682,7 @@
         <v>0.11897000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -692,7 +690,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -706,7 +704,7 @@
         <v>1.1E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -720,7 +718,7 @@
         <v>1.5E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -734,7 +732,7 @@
         <v>1.3000000000000001E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -748,7 +746,7 @@
         <v>3.9E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -756,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -767,7 +765,7 @@
         <v>5.6649999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -781,7 +779,7 @@
         <v>1.3799999999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -795,7 +793,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -809,7 +807,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -823,7 +821,7 @@
         <v>6.9999999999999998E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -832,7 +830,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -841,7 +839,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -850,7 +848,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -859,7 +857,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -867,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -878,7 +876,7 @@
         <v>5.1569999999999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -892,7 +890,7 @@
         <v>2.1800000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -906,7 +904,7 @@
         <v>7.7999999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -920,7 +918,7 @@
         <v>5.6999999999999996E-6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -934,7 +932,7 @@
         <v>8.6999999999999997E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -942,7 +940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -950,7 +948,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -958,7 +956,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -966,7 +964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -974,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -982,7 +980,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -990,7 +988,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -998,7 +996,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1009,7 +1007,7 @@
         <v>5.1490000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1017,7 +1015,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1031,7 +1029,7 @@
         <v>3.7499999999999999E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1045,7 +1043,7 @@
         <v>2.2499999999999998E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1073,7 +1071,7 @@
         <v>5.1999999999999995E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1095,13 +1093,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDCFFEB-8725-4161-8E76-261174ABD25C}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C8" sqref="C8:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1139,7 +1137,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1147,7 +1145,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1158,7 +1156,7 @@
         <v>9.5589999999999994E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1180,7 +1178,7 @@
         <v>7.4700000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1194,7 +1192,7 @@
         <v>8.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1208,7 +1206,7 @@
         <v>3.3000000000000003E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1222,7 +1220,7 @@
         <v>6.8000000000000001E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1230,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1238,7 +1236,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1246,7 +1244,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1254,7 +1252,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1265,7 +1263,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1273,7 +1271,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1287,7 +1285,7 @@
         <v>6.9999999999999994E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>2.0999999999999998E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1315,7 +1313,7 @@
         <v>7.7999999999999997E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1329,7 +1327,7 @@
         <v>3.5999999999999998E-11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1337,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1345,7 +1343,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1353,7 +1351,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1361,7 +1359,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1372,7 +1370,7 @@
         <v>0.45243</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1380,7 +1378,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1394,7 +1392,7 @@
         <v>2.1700000000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1408,7 +1406,7 @@
         <v>1.2160000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1422,7 +1420,7 @@
         <v>2.7299999999999998E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1436,7 +1434,7 @@
         <v>1.3999999999999999E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1444,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1452,7 +1450,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1460,7 +1458,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1468,7 +1466,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1479,7 +1477,7 @@
         <v>0.82310000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1498,7 +1496,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1512,7 +1510,7 @@
         <v>9.1999999999999998E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1526,7 +1524,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1540,7 +1538,7 @@
         <v>7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1562,13 +1560,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCF1270-D6B1-44C8-A245-F6F705039051}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D51" sqref="D2:D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1602,7 +1600,7 @@
         <v>0.40809069999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1617,7 @@
         <v>3.4364050000000002E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1636,7 +1634,7 @@
         <v>3.467936E-15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1653,7 +1651,7 @@
         <v>3.833261E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1670,7 +1668,7 @@
         <v>0.78702609999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1687,7 +1685,7 @@
         <v>1.3624100000000001E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1704,7 +1702,7 @@
         <v>0.33553470000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>1.6746029999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1738,7 +1736,7 @@
         <v>2.125575E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1755,7 +1753,7 @@
         <v>8.1963490000000003E-7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1772,7 +1770,7 @@
         <v>8.1435860000000001E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1789,7 +1787,7 @@
         <v>6.1980059999999995E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>2.9405339999999999E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1823,7 +1821,7 @@
         <v>0.40955970000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1840,7 +1838,7 @@
         <v>0.32968989999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1857,7 +1855,7 @@
         <v>0.36324899999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1874,7 +1872,7 @@
         <v>2.0605279999999999E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1891,7 +1889,7 @@
         <v>2.2171970000000002E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1908,7 +1906,7 @@
         <v>0.59890060000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1925,7 +1923,7 @@
         <v>0.39445069999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1942,7 +1940,7 @@
         <v>0.1000716</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1959,7 +1957,7 @@
         <v>8.6216759999999998E-13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1976,7 +1974,7 @@
         <v>1.5067570000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1993,7 +1991,7 @@
         <v>0.73068500000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2010,7 +2008,7 @@
         <v>0.71914230000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2025,7 @@
         <v>0.40809069999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2044,7 +2042,7 @@
         <v>3.4364050000000002E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2061,7 +2059,7 @@
         <v>3.467936E-15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2078,7 +2076,7 @@
         <v>3.833261E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2095,7 +2093,7 @@
         <v>0.78702609999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2112,7 +2110,7 @@
         <v>1.3624100000000001E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2129,7 +2127,7 @@
         <v>0.33553470000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2146,7 +2144,7 @@
         <v>1.6746029999999999E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>2.125575E-7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2180,7 +2178,7 @@
         <v>8.1963490000000003E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -2197,7 +2195,7 @@
         <v>8.1435860000000001E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -2214,7 +2212,7 @@
         <v>6.1980059999999995E-10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2231,7 +2229,7 @@
         <v>2.9405339999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -2245,7 +2243,7 @@
         <v>0.40955970000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2262,7 +2260,7 @@
         <v>0.32968989999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2279,7 +2277,7 @@
         <v>0.36324899999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2296,7 +2294,7 @@
         <v>2.0605279999999999E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2313,7 +2311,7 @@
         <v>2.2171970000000002E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2327,7 +2325,7 @@
         <v>0.59890060000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2344,7 +2342,7 @@
         <v>0.39445069999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2361,7 +2359,7 @@
         <v>0.1000716</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4</v>
       </c>
@@ -2378,7 +2376,7 @@
         <v>8.6216759999999998E-13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
@@ -2395,7 +2393,7 @@
         <v>1.5067570000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4</v>
       </c>
@@ -2409,7 +2407,7 @@
         <v>0.73068500000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2444,12 +2442,12 @@
       <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2463,7 +2461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2492,7 +2490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2546,7 +2544,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2663,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2684,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -2705,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2726,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2740,7 +2738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2766,7 +2764,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2796,7 +2794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -2824,7 +2822,7 @@
       </c>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2852,7 +2850,7 @@
       </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2880,7 +2878,7 @@
       </c>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2903,7 +2901,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2926,7 +2924,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -2949,7 +2947,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2972,7 +2970,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2995,7 +2993,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3018,7 +3016,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3032,7 +3030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -3061,7 +3059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E27" s="3" t="s">
         <v>33</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E28" s="3" t="s">
         <v>24</v>
       </c>
@@ -3101,7 +3099,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E29" s="3" t="s">
         <v>25</v>
       </c>
@@ -3120,7 +3118,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E30" s="3" t="s">
         <v>26</v>
       </c>
@@ -3139,7 +3137,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E31" s="3" t="s">
         <v>27</v>
       </c>
@@ -3153,7 +3151,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E32" s="2" t="s">
         <v>28</v>
       </c>
@@ -3167,7 +3165,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E33" s="3" t="s">
         <v>29</v>
       </c>
@@ -3181,7 +3179,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E34" s="3" t="s">
         <v>30</v>
       </c>
@@ -3195,7 +3193,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
@@ -3209,7 +3207,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>32</v>
       </c>
@@ -3223,14 +3221,14 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
         <v>40</v>
       </c>
@@ -3250,7 +3248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>33</v>
       </c>
@@ -3271,7 +3269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>24</v>
       </c>
@@ -3289,7 +3287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
         <v>25</v>
       </c>
@@ -3307,7 +3305,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
         <v>26</v>
       </c>
@@ -3325,7 +3323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
         <v>27</v>
       </c>
@@ -3338,7 +3336,7 @@
       </c>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E44" s="2" t="s">
         <v>28</v>
       </c>
@@ -3351,7 +3349,7 @@
       </c>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
         <v>29</v>
       </c>
@@ -3364,7 +3362,7 @@
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
         <v>30</v>
       </c>
@@ -3377,7 +3375,7 @@
       </c>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E47" s="2" t="s">
         <v>31</v>
       </c>
@@ -3390,7 +3388,7 @@
       </c>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E48" s="2" t="s">
         <v>32</v>
       </c>
@@ -3402,14 +3400,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E50" t="s">
         <v>40</v>
       </c>
@@ -3429,7 +3427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E51" t="s">
         <v>33</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
         <v>24</v>
       </c>
@@ -3468,7 +3466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E53" t="s">
         <v>25</v>
       </c>
@@ -3486,7 +3484,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
         <v>26</v>
       </c>
@@ -3504,7 +3502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E55" t="s">
         <v>27</v>
       </c>
@@ -3516,7 +3514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E56" s="2" t="s">
         <v>28</v>
       </c>
@@ -3528,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
         <v>29</v>
       </c>
@@ -3540,7 +3538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
         <v>30</v>
       </c>
@@ -3552,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E59" s="2" t="s">
         <v>31</v>
       </c>
@@ -3564,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E60" s="2" t="s">
         <v>32</v>
       </c>
@@ -3585,16 +3583,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A9EFDD-B5BD-4E5D-8AF1-715EB62FA46E}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3618,7 +3616,6 @@
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="7"/>
       <c r="E2" t="s">
         <v>40</v>
       </c>
@@ -3638,7 +3635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3648,7 +3645,6 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="7"/>
       <c r="E3" t="s">
         <v>33</v>
       </c>
@@ -3666,7 +3662,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3676,7 +3672,6 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="7"/>
       <c r="E4" t="s">
         <v>24</v>
       </c>
@@ -3694,7 +3689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3704,7 +3699,6 @@
       <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="7"/>
       <c r="E5" t="s">
         <v>25</v>
       </c>
@@ -3722,7 +3716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -3732,7 +3726,6 @@
       <c r="C6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="7"/>
       <c r="E6" t="s">
         <v>26</v>
       </c>
@@ -3750,7 +3743,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -3760,7 +3753,6 @@
       <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="7"/>
       <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3772,7 +3764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -3782,7 +3774,6 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7"/>
       <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
@@ -3794,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3804,7 +3795,6 @@
       <c r="C9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="7"/>
       <c r="E9" t="s">
         <v>29</v>
       </c>
@@ -3816,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3826,7 +3816,6 @@
       <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="7"/>
       <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
@@ -3838,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -3848,7 +3837,6 @@
       <c r="C11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="7"/>
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
@@ -3860,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3870,7 +3858,6 @@
       <c r="C12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="7"/>
       <c r="E12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3882,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -3892,14 +3879,13 @@
       <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="7"/>
       <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3909,7 +3895,7 @@
       <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>40</v>
       </c>
@@ -3929,14 +3915,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="1"/>
       <c r="E15" t="s">
         <v>33</v>
       </c>
@@ -3954,7 +3940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3950,6 @@
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="7"/>
       <c r="E16" t="s">
         <v>24</v>
       </c>
@@ -3982,7 +3967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -3992,7 +3977,6 @@
       <c r="C17" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="7"/>
       <c r="E17" s="2" t="s">
         <v>25</v>
       </c>
@@ -4010,7 +3994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4020,7 +4004,7 @@
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="1"/>
       <c r="E18" t="s">
         <v>26</v>
       </c>
@@ -4038,7 +4022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -4048,7 +4032,7 @@
       <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="2" t="s">
         <v>27</v>
       </c>
@@ -4060,14 +4044,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="2" t="s">
         <v>28</v>
       </c>
@@ -4079,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -4089,7 +4073,6 @@
       <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="7"/>
       <c r="E21" t="s">
         <v>29</v>
       </c>
@@ -4101,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4111,7 +4094,6 @@
       <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="7"/>
       <c r="E22" s="2" t="s">
         <v>30</v>
       </c>
@@ -4123,7 +4105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -4133,7 +4115,7 @@
       <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="2" t="s">
         <v>31</v>
       </c>
@@ -4145,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -4155,7 +4137,7 @@
       <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
         <v>32</v>
       </c>
@@ -4167,19 +4149,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="1"/>
       <c r="E25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -4189,7 +4171,6 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="7"/>
       <c r="E26" t="s">
         <v>40</v>
       </c>
@@ -4209,7 +4190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>33</v>
       </c>
@@ -4227,7 +4208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>24</v>
       </c>
@@ -4245,7 +4226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E29" s="2" t="s">
         <v>25</v>
       </c>
@@ -4263,7 +4244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>26</v>
       </c>
@@ -4281,7 +4262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E31" s="2" t="s">
         <v>27</v>
       </c>
@@ -4293,7 +4274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E32" s="2" t="s">
         <v>28</v>
       </c>
@@ -4305,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>29</v>
       </c>
@@ -4317,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E34" s="2" t="s">
         <v>30</v>
       </c>
@@ -4329,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>31</v>
       </c>
@@ -4344,7 +4325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>32</v>
       </c>

</xml_diff>